<commit_message>
add function in csv
</commit_message>
<xml_diff>
--- a/individual hits analysis_yeast_1.xlsx
+++ b/individual hits analysis_yeast_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chee8\Dropbox\BiologyProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BiologyProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="262">
   <si>
     <t>YER030W</t>
   </si>
@@ -430,9 +430,6 @@
   </si>
   <si>
     <t>Paper title</t>
-  </si>
-  <si>
-    <t>Name</t>
   </si>
   <si>
     <t>microtubules stability</t>
@@ -830,6 +827,14 @@
   </si>
   <si>
     <t>LfcinB_unique_2SD</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Molecular function</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -1196,24 +1201,27 @@
   <dimension ref="A1:K64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:K1048576"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.35546875" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" customWidth="1"/>
+    <col min="3" max="3" width="76.42578125" customWidth="1"/>
     <col min="6" max="6" width="29.85546875" customWidth="1"/>
     <col min="11" max="11" width="27.35546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B1" t="s">
         <v>260</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>135</v>
+        <v>261</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>134</v>
@@ -1235,7 +1243,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>127</v>
@@ -1248,7 +1256,7 @@
         <v>126</v>
       </c>
       <c r="I3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
@@ -1256,7 +1264,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C4" t="s">
         <v>128</v>
@@ -1273,7 +1281,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C5" t="s">
         <v>131</v>
@@ -1287,13 +1295,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C6" t="s">
         <v>133</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
@@ -1301,13 +1309,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" t="s">
         <v>142</v>
       </c>
-      <c r="C7" t="s">
+      <c r="G7" t="s">
         <v>143</v>
-      </c>
-      <c r="G7" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
@@ -1315,19 +1323,19 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="G8" s="2" t="s">
+      <c r="I8" t="s">
         <v>146</v>
-      </c>
-      <c r="I8" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
@@ -1335,16 +1343,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G9" t="s">
         <v>150</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="G9" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
@@ -1352,19 +1360,19 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C10" t="s">
+        <v>153</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C10" t="s">
+      <c r="G10" t="s">
         <v>154</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="I10" t="s">
         <v>157</v>
-      </c>
-      <c r="G10" t="s">
-        <v>155</v>
-      </c>
-      <c r="I10" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
@@ -1372,16 +1380,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>160</v>
+      </c>
+      <c r="C11" t="s">
+        <v>158</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C11" t="s">
+      <c r="I11" t="s">
         <v>159</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="I11" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
@@ -1389,19 +1397,19 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C12" t="s">
+        <v>162</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="G12" t="s">
+        <v>165</v>
+      </c>
+      <c r="I12" t="s">
         <v>164</v>
-      </c>
-      <c r="G12" t="s">
-        <v>166</v>
-      </c>
-      <c r="I12" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
@@ -1409,16 +1417,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>169</v>
+      </c>
+      <c r="C13" t="s">
+        <v>167</v>
+      </c>
+      <c r="G13" t="s">
+        <v>168</v>
+      </c>
+      <c r="I13" t="s">
         <v>170</v>
-      </c>
-      <c r="C13" t="s">
-        <v>168</v>
-      </c>
-      <c r="G13" t="s">
-        <v>169</v>
-      </c>
-      <c r="I13" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
@@ -1426,16 +1434,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
+        <v>173</v>
+      </c>
+      <c r="C14" t="s">
+        <v>171</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G14" t="s">
         <v>174</v>
-      </c>
-      <c r="C14" t="s">
-        <v>172</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="G14" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
@@ -1443,13 +1451,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C15" t="s">
+        <v>175</v>
+      </c>
+      <c r="G15" t="s">
         <v>176</v>
-      </c>
-      <c r="G15" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
@@ -1457,16 +1465,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>180</v>
+      </c>
+      <c r="C16" t="s">
+        <v>178</v>
+      </c>
+      <c r="G16" t="s">
+        <v>179</v>
+      </c>
+      <c r="I16" t="s">
         <v>181</v>
-      </c>
-      <c r="C16" t="s">
-        <v>179</v>
-      </c>
-      <c r="G16" t="s">
-        <v>180</v>
-      </c>
-      <c r="I16" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.45">
@@ -1474,13 +1482,13 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
+        <v>182</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="G17" t="s">
         <v>183</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="G17" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.45">
@@ -1488,13 +1496,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C18" t="s">
+        <v>185</v>
+      </c>
+      <c r="G18" t="s">
         <v>186</v>
-      </c>
-      <c r="G18" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.45">
@@ -1502,19 +1510,19 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
+        <v>190</v>
+      </c>
+      <c r="C19" t="s">
+        <v>188</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="G19" t="s">
+        <v>189</v>
+      </c>
+      <c r="I19" t="s">
         <v>191</v>
-      </c>
-      <c r="C19" t="s">
-        <v>189</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="G19" t="s">
-        <v>190</v>
-      </c>
-      <c r="I19" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.45">
@@ -1522,22 +1530,22 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
+        <v>196</v>
+      </c>
+      <c r="C20" t="s">
+        <v>193</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C20" t="s">
+      <c r="G20" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="I20" t="s">
         <v>194</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="K20" t="s">
         <v>198</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="I20" t="s">
-        <v>195</v>
-      </c>
-      <c r="K20" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.45">
@@ -1545,19 +1553,19 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
+        <v>201</v>
+      </c>
+      <c r="C21" t="s">
+        <v>199</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="C21" t="s">
+      <c r="G21" t="s">
+        <v>203</v>
+      </c>
+      <c r="I21" t="s">
         <v>200</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="G21" t="s">
-        <v>204</v>
-      </c>
-      <c r="I21" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.45">
@@ -1565,19 +1573,19 @@
         <v>20</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C22" t="s">
+        <v>204</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="I22" t="s">
+        <v>205</v>
+      </c>
+      <c r="K22" t="s">
         <v>207</v>
-      </c>
-      <c r="C22" t="s">
-        <v>205</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="I22" t="s">
-        <v>206</v>
-      </c>
-      <c r="K22" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.45">
@@ -1585,19 +1593,19 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
+        <v>211</v>
+      </c>
+      <c r="C23" t="s">
+        <v>209</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="C23" t="s">
+      <c r="G23" t="s">
+        <v>213</v>
+      </c>
+      <c r="I23" t="s">
         <v>210</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="G23" t="s">
-        <v>214</v>
-      </c>
-      <c r="I23" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.45">
@@ -1605,16 +1613,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C24" t="s">
+        <v>214</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="I24" t="s">
         <v>215</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="I24" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.45">
@@ -1622,22 +1630,22 @@
         <v>23</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C25" t="s">
+        <v>218</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="G25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I25" t="s">
         <v>219</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="K25" t="s">
         <v>222</v>
-      </c>
-      <c r="G25" t="s">
-        <v>221</v>
-      </c>
-      <c r="I25" t="s">
-        <v>220</v>
-      </c>
-      <c r="K25" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.45">
@@ -1645,19 +1653,19 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
+        <v>226</v>
+      </c>
+      <c r="C26" t="s">
+        <v>224</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="C26" t="s">
+      <c r="G26" t="s">
+        <v>228</v>
+      </c>
+      <c r="I26" t="s">
         <v>225</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="G26" t="s">
-        <v>229</v>
-      </c>
-      <c r="I26" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.45">
@@ -1665,19 +1673,19 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C27" t="s">
+        <v>229</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="G27" t="s">
+        <v>231</v>
+      </c>
+      <c r="I27" t="s">
         <v>230</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="G27" t="s">
-        <v>232</v>
-      </c>
-      <c r="I27" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.45">
@@ -1685,19 +1693,19 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C28" t="s">
+        <v>233</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="G28" t="s">
+        <v>235</v>
+      </c>
+      <c r="I28" t="s">
         <v>234</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="G28" t="s">
-        <v>236</v>
-      </c>
-      <c r="I28" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.45">
@@ -1705,16 +1713,16 @@
         <v>27</v>
       </c>
       <c r="C29" t="s">
+        <v>237</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="I29" t="s">
         <v>238</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="I29" t="s">
+      <c r="K29" t="s">
         <v>239</v>
-      </c>
-      <c r="K29" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.45">
@@ -1722,19 +1730,19 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
+        <v>243</v>
+      </c>
+      <c r="C30" t="s">
+        <v>241</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="G30" t="s">
         <v>244</v>
       </c>
-      <c r="C30" t="s">
+      <c r="I30" t="s">
         <v>242</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="G30" t="s">
-        <v>245</v>
-      </c>
-      <c r="I30" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.45">
@@ -1742,16 +1750,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C31" t="s">
+        <v>246</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="I31" t="s">
         <v>247</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="I31" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.45">
@@ -1759,22 +1767,22 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C32" t="s">
+        <v>249</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="G32" t="s">
+        <v>252</v>
+      </c>
+      <c r="I32" t="s">
         <v>250</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="G32" t="s">
+      <c r="K32" t="s">
         <v>253</v>
-      </c>
-      <c r="I32" t="s">
-        <v>251</v>
-      </c>
-      <c r="K32" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.45">
@@ -1782,16 +1790,16 @@
         <v>31</v>
       </c>
       <c r="C33" t="s">
+        <v>255</v>
+      </c>
+      <c r="E33" t="s">
+        <v>258</v>
+      </c>
+      <c r="I33" t="s">
         <v>256</v>
       </c>
-      <c r="E33" t="s">
-        <v>259</v>
-      </c>
-      <c r="I33" t="s">
+      <c r="K33" t="s">
         <v>257</v>
-      </c>
-      <c r="K33" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.45">

</xml_diff>